<commit_message>
Anonymized output for submission.
</commit_message>
<xml_diff>
--- a/results/Tbl1.xlsx
+++ b/results/Tbl1.xlsx
@@ -42,9 +42,6 @@
     <t>Risk Perception</t>
   </si>
   <si>
-    <t>3-item survey scale (COVIDiStress)</t>
-  </si>
-  <si>
     <t>SE of Risk Perception by Country</t>
   </si>
   <si>
@@ -105,14 +102,41 @@
     <t>Variable</t>
   </si>
   <si>
-    <t>Ratio of infection, May 31st to 1st</t>
+    <r>
+      <t xml:space="preserve">3-item survey scale (COVIDiStress);                              </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>First Stage Dependent Variable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ratio of infection rate, May 31st to 1st, (Johns Hopkins, 18-day lead in COVID-19 deaths); </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Second Stage Dependent Variable</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +272,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
@@ -621,7 +659,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -652,6 +690,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -980,15 +1024,15 @@
       <selection sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="1" customWidth="1"/>
-    <col min="3" max="7" width="5.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="1" customWidth="1"/>
+    <col min="3" max="7" width="5.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="7.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -997,9 +1041,9 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -1020,12 +1064,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3">
         <v>4.5</v>
@@ -1043,12 +1087,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="9">
         <v>0.1</v>
@@ -1066,12 +1110,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="3">
         <v>31.28</v>
@@ -1089,12 +1133,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="C6" s="9">
         <v>0.37</v>
@@ -1112,12 +1156,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -1135,9 +1179,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>16</v>
+    <row r="8" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>28</v>
@@ -1158,12 +1202,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C9" s="3">
         <v>0.23</v>
@@ -1181,12 +1225,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="C10" s="9">
         <v>34.85</v>
@@ -1204,12 +1248,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>0.12</v>
@@ -1227,12 +1271,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="C12" s="9">
         <v>0.62</v>
@@ -1250,12 +1294,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C13" s="6">
         <v>26.17</v>

</xml_diff>